<commit_message>
falsely high FP 1996-98 fixed. need outage RIHT removal from PLNGS data
</commit_message>
<xml_diff>
--- a/FACModel/PLNGS_Power.xlsx
+++ b/FACModel/PLNGS_Power.xlsx
@@ -418,7 +418,7 @@
         <v>35155</v>
       </c>
       <c r="B4">
-        <v>1.011831139845917</v>
+        <v>0.9965793528505477</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -426,7 +426,7 @@
         <v>35185</v>
       </c>
       <c r="B5">
-        <v>1.075611547668067</v>
+        <v>0.9964873949579883</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -434,7 +434,7 @@
         <v>35216</v>
       </c>
       <c r="B6">
-        <v>1.122910578418773</v>
+        <v>0.997342960288812</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -442,7 +442,7 @@
         <v>35246</v>
       </c>
       <c r="B7">
-        <v>1.152851324051021</v>
+        <v>0.9979183673469387</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -450,7 +450,7 @@
         <v>35277</v>
       </c>
       <c r="B8">
-        <v>1.16263258</v>
+        <v>0.9991652173913045</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -458,7 +458,7 @@
         <v>35308</v>
       </c>
       <c r="B9">
-        <v>1.16263258</v>
+        <v>0.9991652173913045</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -466,7 +466,7 @@
         <v>35338</v>
       </c>
       <c r="B10">
-        <v>1.171173958338028</v>
+        <v>0.5072535211267616</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -474,7 +474,7 @@
         <v>35369</v>
       </c>
       <c r="B11">
-        <v>1.171173958338028</v>
+        <v>0.5072535211267616</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -482,7 +482,7 @@
         <v>35399</v>
       </c>
       <c r="B12">
-        <v>1.18325128365625</v>
+        <v>0.8708958333333322</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -490,7 +490,7 @@
         <v>35430</v>
       </c>
       <c r="B13">
-        <v>1.219024045751278</v>
+        <v>0.9943321976149965</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -498,7 +498,7 @@
         <v>35461</v>
       </c>
       <c r="B14">
-        <v>0.6510266695165746</v>
+        <v>0.5103176795580103</v>
       </c>
     </row>
     <row r="15" spans="1:2">

</xml_diff>